<commit_message>
Update TeamAlpha - Progress Sheet.xlsx
</commit_message>
<xml_diff>
--- a/Process/Process Sheet/TeamAlpha - Progress Sheet.xlsx
+++ b/Process/Process Sheet/TeamAlpha - Progress Sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25207"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8C3B99C-8E1D-4448-B457-4F3EDCD681E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4766390-40CB-4AD7-AB58-58CA70AC386D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOM" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Day 4" sheetId="7" r:id="rId6"/>
     <sheet name="Day 5" sheetId="8" r:id="rId7"/>
     <sheet name="Day 6(09-04-2022)" sheetId="9" r:id="rId8"/>
-    <sheet name="Day 7" sheetId="10" r:id="rId9"/>
+    <sheet name="Day 7(11-04-2022)" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="538">
   <si>
     <t>MOM</t>
   </si>
@@ -1553,6 +1553,102 @@
   </si>
   <si>
     <t xml:space="preserve">As a interviewer I should able to logout </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                    -</t>
+  </si>
+  <si>
+    <t>I am in Home Page,When i click on current drive details to view the details and also cancel the drive</t>
+  </si>
+  <si>
+    <t>I am in Home Page,When i click on Scheduled drive details to view the details and also cancel the drive</t>
+  </si>
+  <si>
+    <t>To access this operation I need to be logged in as TAC</t>
+  </si>
+  <si>
+    <t>I am in Home Page,When i click on Upcoming drive details to view the details and also view the response</t>
+  </si>
+  <si>
+    <t>MANAGEMENT</t>
+  </si>
+  <si>
+    <t>To register I must fill all the mandatory fields in the details</t>
+  </si>
+  <si>
+    <t>To access my profile ,first I need to login</t>
+  </si>
+  <si>
+    <t>To recieve notification from TAC ,I need to be verified</t>
+  </si>
+  <si>
+    <t>To recieve Login Credentials from TAC,I need to register</t>
+  </si>
+  <si>
+    <t>To access the application ,I need to login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To access the application ,I need to login </t>
+  </si>
+  <si>
+    <t>I am in Home page,When i click on  Scheduled interviews I Should able to view Scheduled interviews</t>
+  </si>
+  <si>
+    <t>I am Viewing my Scheduled interview,When i click on Cancel ,My interview would be rescheduled</t>
+  </si>
+  <si>
+    <t>I am Viewing my Scheduled interview,When i click on Cancel ,I should able to Mention reasons for Cancellation.</t>
+  </si>
+  <si>
+    <t>To fill reasons for cancellation,I should  first cancel the scheduled interview</t>
+  </si>
+  <si>
+    <t>I am in Navigation bar,When i click on Profile I should able to view and edit my profile</t>
+  </si>
+  <si>
+    <t>To view a profile ,I should  login.</t>
+  </si>
+  <si>
+    <t>I am in Navigation bar,When i click on DashBoard,I should able to see my Consolidated performance</t>
+  </si>
+  <si>
+    <t>To view Dashboard ,I should login.</t>
+  </si>
+  <si>
+    <t>I am in Dashboard,When i click on Total No. of Drives Scheduled  I should able to view my Total No. of Drives Scheduled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To  view Consolidated Performance ,I should have accepted drive invites </t>
+  </si>
+  <si>
+    <t>I am in Dashboard,When i click on Interviews Attended I should able to view my Interviews Attended</t>
+  </si>
+  <si>
+    <t>To veiw Interviews Attended ,I should have attended scheduled interviews</t>
+  </si>
+  <si>
+    <t>I am in Dashboard,When i click on Interviews Denied  I should able to view my Interviews Denied</t>
+  </si>
+  <si>
+    <t>To View Interviews Denied ,I should have denied interviews</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am in Dashboard,When i click on Interviews Ignored  I should able to view my Interviews Ignored </t>
+  </si>
+  <si>
+    <t>To veiw Interviews Ignored, I should not have responded to drive invites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am in Dashboard,When i click on Unused Slots  I should able to view my  Unused Slots  </t>
+  </si>
+  <si>
+    <t>To view Unused slots,I should have given my availability but TAC  has not utilized me</t>
+  </si>
+  <si>
+    <t>I am in Dashboard,When i click on Logout I should be able to LOG OUT</t>
+  </si>
+  <si>
+    <t>To Log out,I need to LOG IN</t>
   </si>
 </sst>
 </file>
@@ -1955,7 +2051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2362,6 +2458,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3152,10 +3251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46290B07-6E6D-4B19-9A9B-C3E38C6518F8}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3745,7 +3844,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:3">
       <c r="A81" s="113">
         <v>4</v>
       </c>
@@ -3753,7 +3852,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:3">
       <c r="A82" s="25">
         <v>5</v>
       </c>
@@ -3761,12 +3860,28 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:3">
       <c r="A83" s="45"/>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:3">
       <c r="A84" s="44" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="114" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" s="39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -9455,7 +9570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F93FD05-AC39-402B-8019-D230876DF7A9}">
   <dimension ref="A1:J241"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A225" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -11061,7 +11176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE4E2DC-7D28-43FA-884A-18B48EC48975}">
   <dimension ref="A4:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D29" workbookViewId="0">
       <selection activeCell="E6" sqref="E6:E16"/>
     </sheetView>
   </sheetViews>
@@ -12292,8 +12407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2905983-969D-4AD4-B72B-B97CB8F99111}">
   <dimension ref="B5:K55"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13323,12 +13438,1051 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF84FF66-0AA3-4B94-BE56-4DE17E29EB86}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F15" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="91.28515625" customWidth="1"/>
+    <col min="6" max="6" width="106.85546875" customWidth="1"/>
+    <col min="7" max="7" width="85.28515625" customWidth="1"/>
+    <col min="8" max="8" width="95.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="18.75">
+      <c r="C2" s="53"/>
+      <c r="D2" s="54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18.75">
+      <c r="C3" s="53"/>
+      <c r="D3" s="55"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75">
+      <c r="C4" s="53"/>
+      <c r="D4" s="56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75">
+      <c r="A5" s="118" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="116" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="116" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="161" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="161" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="117" t="s">
+        <v>220</v>
+      </c>
+      <c r="G5" s="156" t="s">
+        <v>221</v>
+      </c>
+      <c r="H5" s="117" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75">
+      <c r="A6" s="162">
+        <v>1</v>
+      </c>
+      <c r="B6" s="163" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" s="63">
+        <v>1</v>
+      </c>
+      <c r="D6" s="166" t="s">
+        <v>429</v>
+      </c>
+      <c r="E6" s="166" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G6" s="105" t="s">
+        <v>369</v>
+      </c>
+      <c r="H6" s="122" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="148">
+        <v>2</v>
+      </c>
+      <c r="B7" s="148" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="164">
+        <v>2</v>
+      </c>
+      <c r="D7" s="101" t="s">
+        <v>431</v>
+      </c>
+      <c r="E7" s="101" t="s">
+        <v>368</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="G7" s="120" t="s">
+        <v>433</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="148"/>
+      <c r="B8" s="148"/>
+      <c r="C8" s="164">
+        <v>3</v>
+      </c>
+      <c r="D8" s="101" t="s">
+        <v>434</v>
+      </c>
+      <c r="E8" s="101" t="s">
+        <v>412</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G8" s="120" t="s">
+        <v>373</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="148"/>
+      <c r="B9" s="148"/>
+      <c r="C9" s="164">
+        <v>4</v>
+      </c>
+      <c r="D9" s="101" t="s">
+        <v>436</v>
+      </c>
+      <c r="E9" s="101" t="s">
+        <v>376</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="G9" s="160" t="s">
+        <v>438</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="148"/>
+      <c r="B10" s="148"/>
+      <c r="C10" s="164">
+        <v>5</v>
+      </c>
+      <c r="D10" s="101" t="s">
+        <v>439</v>
+      </c>
+      <c r="E10" s="101" t="s">
+        <v>379</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="G10" s="120" t="s">
+        <v>380</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="148"/>
+      <c r="B11" s="148"/>
+      <c r="C11" s="164">
+        <v>6</v>
+      </c>
+      <c r="D11" s="101" t="s">
+        <v>441</v>
+      </c>
+      <c r="E11" s="101" t="s">
+        <v>383</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="G11" s="157" t="s">
+        <v>384</v>
+      </c>
+      <c r="H11" s="103" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="148"/>
+      <c r="B12" s="148"/>
+      <c r="C12" s="164">
+        <v>7</v>
+      </c>
+      <c r="D12" s="101" t="s">
+        <v>443</v>
+      </c>
+      <c r="E12" s="101" t="s">
+        <v>391</v>
+      </c>
+      <c r="F12" s="101" t="s">
+        <v>444</v>
+      </c>
+      <c r="G12" s="158" t="s">
+        <v>415</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="148"/>
+      <c r="B13" s="148"/>
+      <c r="C13" s="164">
+        <v>8</v>
+      </c>
+      <c r="D13" s="101" t="s">
+        <v>445</v>
+      </c>
+      <c r="E13" s="101" t="s">
+        <v>395</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="G13" s="160" t="s">
+        <v>438</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="148"/>
+      <c r="B14" s="148"/>
+      <c r="C14" s="164">
+        <v>9</v>
+      </c>
+      <c r="D14" s="101" t="s">
+        <v>447</v>
+      </c>
+      <c r="E14" s="101" t="s">
+        <v>383</v>
+      </c>
+      <c r="F14" s="155" t="s">
+        <v>507</v>
+      </c>
+      <c r="G14" s="158" t="s">
+        <v>427</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="148"/>
+      <c r="B15" s="148"/>
+      <c r="C15" s="164">
+        <v>10</v>
+      </c>
+      <c r="D15" s="101" t="s">
+        <v>448</v>
+      </c>
+      <c r="E15" s="101" t="s">
+        <v>383</v>
+      </c>
+      <c r="F15" s="101" t="s">
+        <v>508</v>
+      </c>
+      <c r="G15" s="158" t="s">
+        <v>509</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="148"/>
+      <c r="B16" s="148"/>
+      <c r="C16" s="164">
+        <v>11</v>
+      </c>
+      <c r="D16" s="101" t="s">
+        <v>449</v>
+      </c>
+      <c r="E16" s="101" t="s">
+        <v>404</v>
+      </c>
+      <c r="F16" s="101" t="s">
+        <v>510</v>
+      </c>
+      <c r="G16" s="158" t="s">
+        <v>509</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="148">
+        <v>3</v>
+      </c>
+      <c r="B17" s="148" t="s">
+        <v>511</v>
+      </c>
+      <c r="C17" s="164">
+        <v>1</v>
+      </c>
+      <c r="D17" s="68" t="s">
+        <v>450</v>
+      </c>
+      <c r="E17" s="68" t="s">
+        <v>233</v>
+      </c>
+      <c r="F17" s="68" t="s">
+        <v>432</v>
+      </c>
+      <c r="G17" s="158" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A18" s="148"/>
+      <c r="B18" s="148"/>
+      <c r="C18" s="164">
+        <v>2</v>
+      </c>
+      <c r="D18" s="76" t="s">
+        <v>451</v>
+      </c>
+      <c r="E18" s="68" t="s">
+        <v>250</v>
+      </c>
+      <c r="F18" s="68" t="s">
+        <v>430</v>
+      </c>
+      <c r="G18" s="120" t="s">
+        <v>251</v>
+      </c>
+      <c r="H18" s="122"/>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A19" s="148"/>
+      <c r="B19" s="148"/>
+      <c r="C19" s="164">
+        <v>3</v>
+      </c>
+      <c r="D19" s="76" t="s">
+        <v>452</v>
+      </c>
+      <c r="E19" s="68" t="s">
+        <v>453</v>
+      </c>
+      <c r="F19" s="68" t="s">
+        <v>435</v>
+      </c>
+      <c r="G19" s="159" t="s">
+        <v>513</v>
+      </c>
+      <c r="H19" s="122"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="148"/>
+      <c r="B20" s="148"/>
+      <c r="C20" s="164">
+        <v>3</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>454</v>
+      </c>
+      <c r="E20" s="68" t="s">
+        <v>254</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>455</v>
+      </c>
+      <c r="G20" s="120" t="s">
+        <v>258</v>
+      </c>
+      <c r="H20" s="101" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="148"/>
+      <c r="B21" s="148"/>
+      <c r="C21" s="164">
+        <v>4</v>
+      </c>
+      <c r="D21" s="68" t="s">
+        <v>456</v>
+      </c>
+      <c r="E21" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="F21" s="68" t="s">
+        <v>457</v>
+      </c>
+      <c r="G21" s="120" t="s">
+        <v>265</v>
+      </c>
+      <c r="H21" s="101" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="148"/>
+      <c r="B22" s="148"/>
+      <c r="C22" s="164">
+        <v>5</v>
+      </c>
+      <c r="D22" s="68" t="s">
+        <v>458</v>
+      </c>
+      <c r="E22" s="68" t="s">
+        <v>268</v>
+      </c>
+      <c r="F22" s="102" t="s">
+        <v>459</v>
+      </c>
+      <c r="G22" s="120" t="s">
+        <v>272</v>
+      </c>
+      <c r="H22" s="101" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="148"/>
+      <c r="B23" s="148"/>
+      <c r="C23" s="164">
+        <v>6</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>460</v>
+      </c>
+      <c r="E23" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>461</v>
+      </c>
+      <c r="G23" s="120" t="s">
+        <v>278</v>
+      </c>
+      <c r="H23" s="101" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="148"/>
+      <c r="B24" s="148"/>
+      <c r="C24" s="164">
+        <v>7</v>
+      </c>
+      <c r="D24" s="70" t="s">
+        <v>462</v>
+      </c>
+      <c r="E24" s="70" t="s">
+        <v>281</v>
+      </c>
+      <c r="F24" s="102" t="s">
+        <v>463</v>
+      </c>
+      <c r="G24" s="120" t="s">
+        <v>285</v>
+      </c>
+      <c r="H24" s="101" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="148"/>
+      <c r="B25" s="148"/>
+      <c r="C25" s="164">
+        <v>8</v>
+      </c>
+      <c r="D25" s="70" t="s">
+        <v>464</v>
+      </c>
+      <c r="E25" s="70" t="s">
+        <v>288</v>
+      </c>
+      <c r="F25" s="68" t="s">
+        <v>465</v>
+      </c>
+      <c r="G25" s="165" t="s">
+        <v>291</v>
+      </c>
+      <c r="H25" s="102" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="148"/>
+      <c r="B26" s="148"/>
+      <c r="C26" s="164">
+        <v>9</v>
+      </c>
+      <c r="D26" s="70" t="s">
+        <v>466</v>
+      </c>
+      <c r="E26" s="70" t="s">
+        <v>294</v>
+      </c>
+      <c r="F26" s="68" t="s">
+        <v>467</v>
+      </c>
+      <c r="G26" s="120" t="s">
+        <v>297</v>
+      </c>
+      <c r="H26" s="102" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="148"/>
+      <c r="B27" s="148"/>
+      <c r="C27" s="164">
+        <v>10</v>
+      </c>
+      <c r="D27" s="70" t="s">
+        <v>468</v>
+      </c>
+      <c r="E27" s="70" t="s">
+        <v>300</v>
+      </c>
+      <c r="F27" s="68" t="s">
+        <v>469</v>
+      </c>
+      <c r="G27" s="120" t="s">
+        <v>304</v>
+      </c>
+      <c r="H27" s="102" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="148"/>
+      <c r="B28" s="148"/>
+      <c r="C28" s="164">
+        <v>11</v>
+      </c>
+      <c r="D28" s="68" t="s">
+        <v>470</v>
+      </c>
+      <c r="E28" s="68" t="s">
+        <v>307</v>
+      </c>
+      <c r="F28" s="102" t="s">
+        <v>471</v>
+      </c>
+      <c r="G28" s="120" t="s">
+        <v>311</v>
+      </c>
+      <c r="H28" s="102" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="148">
+        <v>4</v>
+      </c>
+      <c r="B29" s="148" t="s">
+        <v>313</v>
+      </c>
+      <c r="C29" s="164">
+        <v>1</v>
+      </c>
+      <c r="D29" s="68" t="s">
+        <v>314</v>
+      </c>
+      <c r="E29" s="68" t="s">
+        <v>428</v>
+      </c>
+      <c r="F29" s="68" t="s">
+        <v>472</v>
+      </c>
+      <c r="G29" t="s">
+        <v>514</v>
+      </c>
+      <c r="H29" s="101" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="148"/>
+      <c r="B30" s="148"/>
+      <c r="C30" s="164">
+        <f>(C29+1)</f>
+        <v>2</v>
+      </c>
+      <c r="D30" s="68" t="s">
+        <v>473</v>
+      </c>
+      <c r="E30" s="68" t="s">
+        <v>318</v>
+      </c>
+      <c r="F30" s="68" t="s">
+        <v>474</v>
+      </c>
+      <c r="G30" s="120" t="s">
+        <v>515</v>
+      </c>
+      <c r="H30" s="101"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="148"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="164">
+        <v>3</v>
+      </c>
+      <c r="D31" s="81" t="s">
+        <v>320</v>
+      </c>
+      <c r="E31" s="81" t="s">
+        <v>321</v>
+      </c>
+      <c r="F31" s="102" t="s">
+        <v>475</v>
+      </c>
+      <c r="G31" s="120" t="s">
+        <v>516</v>
+      </c>
+      <c r="H31" s="101"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="148"/>
+      <c r="B32" s="148"/>
+      <c r="C32" s="164">
+        <f t="shared" ref="C32:C50" si="0">(C31+1)</f>
+        <v>4</v>
+      </c>
+      <c r="D32" s="81" t="s">
+        <v>476</v>
+      </c>
+      <c r="E32" s="81" t="s">
+        <v>477</v>
+      </c>
+      <c r="F32" s="102" t="s">
+        <v>475</v>
+      </c>
+      <c r="G32" s="120" t="s">
+        <v>517</v>
+      </c>
+      <c r="H32" s="101"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="148"/>
+      <c r="B33" s="148"/>
+      <c r="C33" s="164">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D33" s="81" t="s">
+        <v>478</v>
+      </c>
+      <c r="E33" s="81" t="s">
+        <v>479</v>
+      </c>
+      <c r="F33" s="102" t="s">
+        <v>480</v>
+      </c>
+      <c r="G33" s="120" t="s">
+        <v>516</v>
+      </c>
+      <c r="H33" s="101"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="148"/>
+      <c r="B34" s="148"/>
+      <c r="C34" s="164">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D34" s="81" t="s">
+        <v>481</v>
+      </c>
+      <c r="E34" s="81" t="s">
+        <v>482</v>
+      </c>
+      <c r="F34" s="102" t="s">
+        <v>483</v>
+      </c>
+      <c r="G34" s="120" t="s">
+        <v>516</v>
+      </c>
+      <c r="H34" s="101"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="148"/>
+      <c r="B35" s="148"/>
+      <c r="C35" s="164">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D35" s="81" t="s">
+        <v>484</v>
+      </c>
+      <c r="E35" s="81" t="s">
+        <v>321</v>
+      </c>
+      <c r="F35" s="102" t="s">
+        <v>485</v>
+      </c>
+      <c r="G35" s="120" t="s">
+        <v>516</v>
+      </c>
+      <c r="H35" s="101"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="148"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="164">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D36" s="70" t="s">
+        <v>324</v>
+      </c>
+      <c r="E36" s="70" t="s">
+        <v>195</v>
+      </c>
+      <c r="F36" s="68" t="s">
+        <v>486</v>
+      </c>
+      <c r="G36" s="120" t="s">
+        <v>516</v>
+      </c>
+      <c r="H36" s="101"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="148"/>
+      <c r="B37" s="148"/>
+      <c r="C37" s="164">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D37" s="102" t="s">
+        <v>487</v>
+      </c>
+      <c r="E37" s="70" t="s">
+        <v>488</v>
+      </c>
+      <c r="F37" s="68" t="s">
+        <v>489</v>
+      </c>
+      <c r="G37" s="120" t="s">
+        <v>516</v>
+      </c>
+      <c r="H37" s="101"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="148"/>
+      <c r="B38" s="148"/>
+      <c r="C38" s="164">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D38" s="102" t="s">
+        <v>490</v>
+      </c>
+      <c r="E38" s="70" t="s">
+        <v>491</v>
+      </c>
+      <c r="F38" s="68" t="s">
+        <v>492</v>
+      </c>
+      <c r="G38" s="120" t="s">
+        <v>516</v>
+      </c>
+      <c r="H38" s="101"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="148"/>
+      <c r="B39" s="148"/>
+      <c r="C39" s="164">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D39" s="70" t="s">
+        <v>328</v>
+      </c>
+      <c r="E39" s="70" t="s">
+        <v>329</v>
+      </c>
+      <c r="F39" s="101" t="s">
+        <v>493</v>
+      </c>
+      <c r="G39" s="106" t="s">
+        <v>494</v>
+      </c>
+      <c r="H39" s="101"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="148"/>
+      <c r="B40" s="148"/>
+      <c r="C40" s="164">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D40" s="70" t="s">
+        <v>495</v>
+      </c>
+      <c r="E40" s="70" t="s">
+        <v>334</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="G40" s="106" t="s">
+        <v>497</v>
+      </c>
+      <c r="H40" s="101"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="148"/>
+      <c r="B41" s="148"/>
+      <c r="C41" s="164">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D41" s="70" t="s">
+        <v>335</v>
+      </c>
+      <c r="E41" s="70" t="s">
+        <v>336</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="G41" s="106" t="s">
+        <v>498</v>
+      </c>
+      <c r="H41" s="101"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="148"/>
+      <c r="B42" s="148"/>
+      <c r="C42" s="164">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D42" s="70" t="s">
+        <v>499</v>
+      </c>
+      <c r="E42" s="70" t="s">
+        <v>500</v>
+      </c>
+      <c r="F42" s="68" t="s">
+        <v>520</v>
+      </c>
+      <c r="G42" s="120" t="s">
+        <v>521</v>
+      </c>
+      <c r="H42" s="101"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="148"/>
+      <c r="B43" s="148"/>
+      <c r="C43" s="164">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D43" s="70" t="s">
+        <v>337</v>
+      </c>
+      <c r="E43" s="70" t="s">
+        <v>338</v>
+      </c>
+      <c r="F43" s="68" t="s">
+        <v>522</v>
+      </c>
+      <c r="G43" s="120" t="s">
+        <v>523</v>
+      </c>
+      <c r="H43" s="101"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="148"/>
+      <c r="B44" s="148"/>
+      <c r="C44" s="164">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D44" s="70" t="s">
+        <v>501</v>
+      </c>
+      <c r="E44" s="70" t="s">
+        <v>502</v>
+      </c>
+      <c r="F44" s="68" t="s">
+        <v>524</v>
+      </c>
+      <c r="G44" s="120" t="s">
+        <v>525</v>
+      </c>
+      <c r="H44" s="101"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="148"/>
+      <c r="B45" s="148"/>
+      <c r="C45" s="164">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D45" s="70" t="s">
+        <v>503</v>
+      </c>
+      <c r="E45" s="70" t="s">
+        <v>342</v>
+      </c>
+      <c r="F45" s="68" t="s">
+        <v>526</v>
+      </c>
+      <c r="G45" s="120" t="s">
+        <v>527</v>
+      </c>
+      <c r="H45" s="101"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="148"/>
+      <c r="B46" s="148"/>
+      <c r="C46" s="164">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D46" s="70" t="s">
+        <v>343</v>
+      </c>
+      <c r="E46" s="70" t="s">
+        <v>281</v>
+      </c>
+      <c r="F46" s="68" t="s">
+        <v>528</v>
+      </c>
+      <c r="G46" s="120" t="s">
+        <v>529</v>
+      </c>
+      <c r="H46" s="101"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="148"/>
+      <c r="B47" s="148"/>
+      <c r="C47" s="164">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D47" s="70" t="s">
+        <v>344</v>
+      </c>
+      <c r="E47" s="70" t="s">
+        <v>288</v>
+      </c>
+      <c r="F47" s="68" t="s">
+        <v>530</v>
+      </c>
+      <c r="G47" s="120" t="s">
+        <v>531</v>
+      </c>
+      <c r="H47" s="101"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="148"/>
+      <c r="B48" s="148"/>
+      <c r="C48" s="164">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D48" s="70" t="s">
+        <v>345</v>
+      </c>
+      <c r="E48" s="70" t="s">
+        <v>294</v>
+      </c>
+      <c r="F48" s="68" t="s">
+        <v>532</v>
+      </c>
+      <c r="G48" s="120" t="s">
+        <v>533</v>
+      </c>
+      <c r="H48" s="101"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="148"/>
+      <c r="B49" s="148"/>
+      <c r="C49" s="164">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D49" s="70" t="s">
+        <v>346</v>
+      </c>
+      <c r="E49" s="70" t="s">
+        <v>504</v>
+      </c>
+      <c r="F49" s="68" t="s">
+        <v>534</v>
+      </c>
+      <c r="G49" s="120" t="s">
+        <v>535</v>
+      </c>
+      <c r="H49" s="101"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="148"/>
+      <c r="B50" s="148"/>
+      <c r="C50" s="164">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D50" s="70" t="s">
+        <v>505</v>
+      </c>
+      <c r="E50" s="70" t="s">
+        <v>347</v>
+      </c>
+      <c r="F50" s="68" t="s">
+        <v>536</v>
+      </c>
+      <c r="G50" s="120" t="s">
+        <v>537</v>
+      </c>
+      <c r="H50" s="101"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A7:A16"/>
+    <mergeCell ref="B7:B16"/>
+    <mergeCell ref="A17:A28"/>
+    <mergeCell ref="B17:B28"/>
+    <mergeCell ref="A29:A50"/>
+    <mergeCell ref="B29:B50"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>